<commit_message>
i had messed up some begins and ands in the spreadsheet around tghe write jumps... I think. Sheet and 4164 4816 delays updated and uf2 rebuilt.
</commit_message>
<xml_diff>
--- a/firmware/timings/Pico Dram Tester Timings.xlsx
+++ b/firmware/timings/Pico Dram Tester Timings.xlsx
@@ -15,7 +15,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="XsKJmh39ZCdJB50Z0P1EcOTGzSiKq3knHahiXgoWTus="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="ZwWgNwQJsgYHF1GbA665rnHutkvt3Le2CocTPx7oyZE="/>
     </ext>
   </extLst>
 </workbook>
@@ -33,7 +33,7 @@
     <t>These sheets share a common format. Everything left and below of D3 should be indentical formulas and formatting.</t>
   </si>
   <si>
-    <t xml:space="preserve">To use a sheet, the idea is to zero out the all the 'Delays' values and then prgressively increase each one in order until all the timing cells between the nop instructions are white. </t>
+    <t xml:space="preserve">To use a sheet, the idea is to zero out the all the 'Delays' values and then progressively increase each one in order until all the timing cells between the relevant nop instructions are white. </t>
   </si>
   <si>
     <t>The conditional formatting is my interpretation of the what the delays between PIO commands need to be. Please let me know what I've missed or got wrong. I've only been learning this stuff for a few days. :-) The conditional formatting looks up the relevant values in the Chip Timings table.</t>
@@ -3321,23 +3321,31 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
         <v>3.0</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
+    <row r="7">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3455,7 +3463,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" ref="G5:G24" si="2">H4</f>
+        <f t="shared" ref="G5:G12" si="2">H4</f>
         <v>19.998</v>
       </c>
       <c r="H5" s="21">
@@ -3524,8 +3532,8 @@
       <c r="A8" s="22">
         <v>4.0</v>
       </c>
-      <c r="B8" s="17">
-        <v>10.0</v>
+      <c r="B8" s="26">
+        <v>12.0</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -3671,12 +3679,12 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="28">
-        <f t="shared" si="2"/>
-        <v>116.655</v>
+        <f>H10</f>
+        <v>109.989</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="1"/>
-        <v>119.988</v>
+        <v>113.322</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>38</v>
@@ -3698,12 +3706,12 @@
         <v>0.0</v>
       </c>
       <c r="G14" s="29">
-        <f t="shared" si="2"/>
-        <v>119.988</v>
+        <f>H13</f>
+        <v>113.322</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>
-        <v>123.321</v>
+        <v>116.655</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>41</v>
@@ -3728,12 +3736,12 @@
         <v>0.0</v>
       </c>
       <c r="G15" s="20">
-        <f t="shared" si="2"/>
-        <v>123.321</v>
+        <f>H12</f>
+        <v>116.655</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="1"/>
-        <v>126.654</v>
+        <v>119.988</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>45</v>
@@ -3755,8 +3763,8 @@
         <v>4.0</v>
       </c>
       <c r="G16" s="20">
-        <f t="shared" si="2"/>
-        <v>126.654</v>
+        <f t="shared" ref="G16:G24" si="3">H15</f>
+        <v>119.988</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="1"/>
@@ -3782,7 +3790,7 @@
         <v>0.0</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>163.317</v>
       </c>
       <c r="H17" s="25">
@@ -3809,7 +3817,7 @@
         <v>0.0</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166.65</v>
       </c>
       <c r="H18" s="21">
@@ -3836,7 +3844,7 @@
         <v>5.0</v>
       </c>
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>169.983</v>
       </c>
       <c r="H19" s="21">
@@ -3863,7 +3871,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>186.648</v>
       </c>
       <c r="H20" s="21">
@@ -3890,7 +3898,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>189.981</v>
       </c>
       <c r="H21" s="21">
@@ -3917,7 +3925,7 @@
         <v>0.0</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>193.314</v>
       </c>
       <c r="H22" s="21">
@@ -3942,7 +3950,7 @@
         <v>6.0</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>196.647</v>
       </c>
       <c r="H23" s="21">
@@ -3969,7 +3977,7 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199.98</v>
       </c>
       <c r="H24" s="21">
@@ -4025,7 +4033,7 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="21">
-        <f t="shared" ref="H26:H30" si="3">G26+(offset($B$4,$F26,0)+1)*3.333</f>
+        <f t="shared" ref="H26:H30" si="4">G26+(offset($B$4,$F26,0)+1)*3.333</f>
         <v>3.333</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -4050,11 +4058,11 @@
         <v>0.0</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" ref="G27:G30" si="4">H26</f>
+        <f t="shared" ref="G27:G30" si="5">H26</f>
         <v>3.333</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666</v>
       </c>
       <c r="I27" s="19"/>
@@ -4075,11 +4083,11 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="20">
+        <f t="shared" si="5"/>
+        <v>6.666</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>6.666</v>
-      </c>
-      <c r="H28" s="21">
-        <f t="shared" si="3"/>
         <v>9.999</v>
       </c>
       <c r="I28" s="19"/>
@@ -4096,11 +4104,11 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="20">
+        <f t="shared" si="5"/>
+        <v>9.999</v>
+      </c>
+      <c r="H29" s="21">
         <f t="shared" si="4"/>
-        <v>9.999</v>
-      </c>
-      <c r="H29" s="21">
-        <f t="shared" si="3"/>
         <v>13.332</v>
       </c>
       <c r="I29" s="19"/>
@@ -4117,11 +4125,11 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="20">
+        <f t="shared" si="5"/>
+        <v>13.332</v>
+      </c>
+      <c r="H30" s="21">
         <f t="shared" si="4"/>
-        <v>13.332</v>
-      </c>
-      <c r="H30" s="21">
-        <f t="shared" si="3"/>
         <v>16.665</v>
       </c>
       <c r="I30" s="19"/>
@@ -5829,7 +5837,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" ref="G5:G24" si="2">H4</f>
+        <f t="shared" ref="G5:G12" si="2">H4</f>
         <v>19.998</v>
       </c>
       <c r="H5" s="21">
@@ -5898,8 +5906,8 @@
       <c r="A8" s="22">
         <v>4.0</v>
       </c>
-      <c r="B8" s="17">
-        <v>15.0</v>
+      <c r="B8" s="26">
+        <v>17.0</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -5925,7 +5933,7 @@
       <c r="A9" s="22">
         <v>5.0</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="26">
         <v>4.0</v>
       </c>
       <c r="C9" s="18"/>
@@ -6045,12 +6053,12 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="28">
-        <f t="shared" si="2"/>
-        <v>129.987</v>
+        <f>H10</f>
+        <v>123.321</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="1"/>
-        <v>133.32</v>
+        <v>126.654</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>88</v>
@@ -6072,12 +6080,12 @@
         <v>0.0</v>
       </c>
       <c r="G14" s="29">
-        <f t="shared" si="2"/>
-        <v>133.32</v>
+        <f>H13</f>
+        <v>126.654</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>
-        <v>136.653</v>
+        <v>129.987</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>41</v>
@@ -6101,12 +6109,12 @@
         <v>0.0</v>
       </c>
       <c r="G15" s="20">
-        <f t="shared" si="2"/>
-        <v>136.653</v>
+        <f>H12</f>
+        <v>129.987</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="1"/>
-        <v>139.986</v>
+        <v>133.32</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>45</v>
@@ -6128,8 +6136,8 @@
         <v>4.0</v>
       </c>
       <c r="G16" s="20">
-        <f t="shared" si="2"/>
-        <v>139.986</v>
+        <f t="shared" ref="G16:G24" si="3">H15</f>
+        <v>133.32</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="1"/>
@@ -6155,7 +6163,7 @@
         <v>0.0</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>193.314</v>
       </c>
       <c r="H17" s="25">
@@ -6182,7 +6190,7 @@
         <v>0.0</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>196.647</v>
       </c>
       <c r="H18" s="21">
@@ -6209,7 +6217,7 @@
         <v>5.0</v>
       </c>
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199.98</v>
       </c>
       <c r="H19" s="21">
@@ -6236,7 +6244,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>216.645</v>
       </c>
       <c r="H20" s="21">
@@ -6263,7 +6271,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>219.978</v>
       </c>
       <c r="H21" s="21">
@@ -6290,7 +6298,7 @@
         <v>0.0</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>223.311</v>
       </c>
       <c r="H22" s="21">
@@ -6315,7 +6323,7 @@
         <v>6.0</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226.644</v>
       </c>
       <c r="H23" s="21">
@@ -6342,7 +6350,7 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>229.977</v>
       </c>
       <c r="H24" s="21">
@@ -6398,7 +6406,7 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="21">
-        <f t="shared" ref="H26:H30" si="3">G26+(offset($B$4,$F26,0)+1)*3.333</f>
+        <f t="shared" ref="H26:H30" si="4">G26+(offset($B$4,$F26,0)+1)*3.333</f>
         <v>3.333</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -6423,11 +6431,11 @@
         <v>0.0</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" ref="G27:G30" si="4">H26</f>
+        <f t="shared" ref="G27:G30" si="5">H26</f>
         <v>3.333</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666</v>
       </c>
       <c r="I27" s="19"/>
@@ -6448,11 +6456,11 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="20">
+        <f t="shared" si="5"/>
+        <v>6.666</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>6.666</v>
-      </c>
-      <c r="H28" s="21">
-        <f t="shared" si="3"/>
         <v>9.999</v>
       </c>
       <c r="I28" s="19"/>
@@ -6469,11 +6477,11 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="20">
+        <f t="shared" si="5"/>
+        <v>9.999</v>
+      </c>
+      <c r="H29" s="21">
         <f t="shared" si="4"/>
-        <v>9.999</v>
-      </c>
-      <c r="H29" s="21">
-        <f t="shared" si="3"/>
         <v>13.332</v>
       </c>
       <c r="I29" s="19"/>
@@ -6490,11 +6498,11 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="20">
+        <f t="shared" si="5"/>
+        <v>13.332</v>
+      </c>
+      <c r="H30" s="21">
         <f t="shared" si="4"/>
-        <v>13.332</v>
-      </c>
-      <c r="H30" s="21">
-        <f t="shared" si="3"/>
         <v>16.665</v>
       </c>
       <c r="I30" s="19"/>
@@ -7693,7 +7701,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" ref="G5:G24" si="2">H4</f>
+        <f t="shared" ref="G5:G12" si="2">H4</f>
         <v>19.998</v>
       </c>
       <c r="H5" s="21">
@@ -7762,8 +7770,8 @@
       <c r="A8" s="22">
         <v>4.0</v>
       </c>
-      <c r="B8" s="17">
-        <v>22.0</v>
+      <c r="B8" s="26">
+        <v>24.0</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -7789,7 +7797,7 @@
       <c r="A9" s="22">
         <v>5.0</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="26">
         <v>6.0</v>
       </c>
       <c r="C9" s="18"/>
@@ -7909,12 +7917,12 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="28">
-        <f t="shared" si="2"/>
-        <v>139.986</v>
+        <f>H10</f>
+        <v>133.32</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="1"/>
-        <v>143.319</v>
+        <v>136.653</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>97</v>
@@ -7936,12 +7944,12 @@
         <v>0.0</v>
       </c>
       <c r="G14" s="29">
-        <f t="shared" si="2"/>
-        <v>143.319</v>
+        <f>H13</f>
+        <v>136.653</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>
-        <v>146.652</v>
+        <v>139.986</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>41</v>
@@ -7965,12 +7973,12 @@
         <v>0.0</v>
       </c>
       <c r="G15" s="20">
-        <f t="shared" si="2"/>
-        <v>146.652</v>
+        <f>H12</f>
+        <v>139.986</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="1"/>
-        <v>149.985</v>
+        <v>143.319</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>45</v>
@@ -7992,8 +8000,8 @@
         <v>4.0</v>
       </c>
       <c r="G16" s="20">
-        <f t="shared" si="2"/>
-        <v>149.985</v>
+        <f t="shared" ref="G16:G24" si="3">H15</f>
+        <v>143.319</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="1"/>
@@ -8019,7 +8027,7 @@
         <v>0.0</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226.644</v>
       </c>
       <c r="H17" s="25">
@@ -8046,7 +8054,7 @@
         <v>0.0</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>229.977</v>
       </c>
       <c r="H18" s="21">
@@ -8073,7 +8081,7 @@
         <v>5.0</v>
       </c>
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>233.31</v>
       </c>
       <c r="H19" s="21">
@@ -8100,7 +8108,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256.641</v>
       </c>
       <c r="H20" s="21">
@@ -8127,7 +8135,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>259.974</v>
       </c>
       <c r="H21" s="21">
@@ -8154,7 +8162,7 @@
         <v>0.0</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>263.307</v>
       </c>
       <c r="H22" s="21">
@@ -8179,7 +8187,7 @@
         <v>6.0</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>266.64</v>
       </c>
       <c r="H23" s="21">
@@ -8206,7 +8214,7 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>269.973</v>
       </c>
       <c r="H24" s="21">
@@ -8262,7 +8270,7 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="21">
-        <f t="shared" ref="H26:H30" si="3">G26+(offset($B$4,$F26,0)+1)*3.333</f>
+        <f t="shared" ref="H26:H30" si="4">G26+(offset($B$4,$F26,0)+1)*3.333</f>
         <v>3.333</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -8287,11 +8295,11 @@
         <v>0.0</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" ref="G27:G30" si="4">H26</f>
+        <f t="shared" ref="G27:G30" si="5">H26</f>
         <v>3.333</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666</v>
       </c>
       <c r="I27" s="19"/>
@@ -8312,11 +8320,11 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="20">
+        <f t="shared" si="5"/>
+        <v>6.666</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>6.666</v>
-      </c>
-      <c r="H28" s="21">
-        <f t="shared" si="3"/>
         <v>9.999</v>
       </c>
       <c r="I28" s="19"/>
@@ -8333,11 +8341,11 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="20">
+        <f t="shared" si="5"/>
+        <v>9.999</v>
+      </c>
+      <c r="H29" s="21">
         <f t="shared" si="4"/>
-        <v>9.999</v>
-      </c>
-      <c r="H29" s="21">
-        <f t="shared" si="3"/>
         <v>13.332</v>
       </c>
       <c r="I29" s="19"/>
@@ -8354,11 +8362,11 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="20">
+        <f t="shared" si="5"/>
+        <v>13.332</v>
+      </c>
+      <c r="H30" s="21">
         <f t="shared" si="4"/>
-        <v>13.332</v>
-      </c>
-      <c r="H30" s="21">
-        <f t="shared" si="3"/>
         <v>16.665</v>
       </c>
       <c r="I30" s="19"/>
@@ -9557,7 +9565,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" ref="G5:G24" si="2">H4</f>
+        <f t="shared" ref="G5:G12" si="2">H4</f>
         <v>19.998</v>
       </c>
       <c r="H5" s="21">
@@ -9599,8 +9607,8 @@
       <c r="A7" s="22">
         <v>3.0</v>
       </c>
-      <c r="B7" s="17">
-        <v>4.0</v>
+      <c r="B7" s="26">
+        <v>5.0</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="17"/>
@@ -9626,8 +9634,8 @@
       <c r="A8" s="22">
         <v>4.0</v>
       </c>
-      <c r="B8" s="17">
-        <v>8.0</v>
+      <c r="B8" s="26">
+        <v>9.0</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -9643,7 +9651,7 @@
       </c>
       <c r="H8" s="21">
         <f t="shared" si="1"/>
-        <v>133.32</v>
+        <v>136.653</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>25</v>
@@ -9653,7 +9661,7 @@
       <c r="A9" s="22">
         <v>5.0</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="26">
         <v>6.0</v>
       </c>
       <c r="C9" s="18"/>
@@ -9668,11 +9676,11 @@
       </c>
       <c r="G9" s="24">
         <f t="shared" si="2"/>
-        <v>133.32</v>
+        <v>136.653</v>
       </c>
       <c r="H9" s="21">
         <f t="shared" si="1"/>
-        <v>136.653</v>
+        <v>139.986</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>104</v>
@@ -9682,7 +9690,7 @@
       <c r="A10" s="22">
         <v>6.0</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="26">
         <v>3.0</v>
       </c>
       <c r="C10" s="18"/>
@@ -9695,11 +9703,11 @@
       </c>
       <c r="G10" s="20">
         <f t="shared" si="2"/>
-        <v>136.653</v>
+        <v>139.986</v>
       </c>
       <c r="H10" s="21">
         <f t="shared" si="1"/>
-        <v>139.986</v>
+        <v>143.319</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>30</v>
@@ -9722,11 +9730,11 @@
       </c>
       <c r="G11" s="24">
         <f t="shared" si="2"/>
-        <v>139.986</v>
+        <v>143.319</v>
       </c>
       <c r="H11" s="25">
         <f t="shared" si="1"/>
-        <v>143.319</v>
+        <v>146.652</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>105</v>
@@ -9747,11 +9755,11 @@
       </c>
       <c r="G12" s="20">
         <f t="shared" si="2"/>
-        <v>143.319</v>
+        <v>146.652</v>
       </c>
       <c r="H12" s="21">
         <f t="shared" si="1"/>
-        <v>146.652</v>
+        <v>149.985</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>34</v>
@@ -9773,12 +9781,12 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="28">
-        <f t="shared" si="2"/>
-        <v>146.652</v>
+        <f>H10</f>
+        <v>143.319</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="1"/>
-        <v>149.985</v>
+        <v>146.652</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>106</v>
@@ -9800,12 +9808,12 @@
         <v>0.0</v>
       </c>
       <c r="G14" s="29">
-        <f t="shared" si="2"/>
-        <v>149.985</v>
+        <f>H13</f>
+        <v>146.652</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>
-        <v>153.318</v>
+        <v>149.985</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>41</v>
@@ -9829,12 +9837,12 @@
         <v>0.0</v>
       </c>
       <c r="G15" s="20">
-        <f t="shared" si="2"/>
-        <v>153.318</v>
+        <f>H12</f>
+        <v>149.985</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="1"/>
-        <v>156.651</v>
+        <v>153.318</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>45</v>
@@ -9856,8 +9864,8 @@
         <v>4.0</v>
       </c>
       <c r="G16" s="20">
-        <f t="shared" si="2"/>
-        <v>156.651</v>
+        <f t="shared" ref="G16:G24" si="3">H15</f>
+        <v>153.318</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="1"/>
@@ -9883,7 +9891,7 @@
         <v>0.0</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>186.648</v>
       </c>
       <c r="H17" s="25">
@@ -9910,7 +9918,7 @@
         <v>0.0</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>189.981</v>
       </c>
       <c r="H18" s="21">
@@ -9937,7 +9945,7 @@
         <v>5.0</v>
       </c>
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>193.314</v>
       </c>
       <c r="H19" s="21">
@@ -9964,7 +9972,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>216.645</v>
       </c>
       <c r="H20" s="21">
@@ -9991,7 +9999,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>219.978</v>
       </c>
       <c r="H21" s="21">
@@ -10018,7 +10026,7 @@
         <v>0.0</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>223.311</v>
       </c>
       <c r="H22" s="21">
@@ -10043,7 +10051,7 @@
         <v>6.0</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226.644</v>
       </c>
       <c r="H23" s="21">
@@ -10070,7 +10078,7 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>239.976</v>
       </c>
       <c r="H24" s="21">
@@ -10126,7 +10134,7 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="21">
-        <f t="shared" ref="H26:H30" si="3">G26+(offset($B$4,$F26,0)+1)*3.333</f>
+        <f t="shared" ref="H26:H30" si="4">G26+(offset($B$4,$F26,0)+1)*3.333</f>
         <v>3.333</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -10151,11 +10159,11 @@
         <v>0.0</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" ref="G27:G30" si="4">H26</f>
+        <f t="shared" ref="G27:G30" si="5">H26</f>
         <v>3.333</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666</v>
       </c>
       <c r="I27" s="19"/>
@@ -10176,11 +10184,11 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="20">
+        <f t="shared" si="5"/>
+        <v>6.666</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>6.666</v>
-      </c>
-      <c r="H28" s="21">
-        <f t="shared" si="3"/>
         <v>9.999</v>
       </c>
       <c r="I28" s="19"/>
@@ -10197,11 +10205,11 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="20">
+        <f t="shared" si="5"/>
+        <v>9.999</v>
+      </c>
+      <c r="H29" s="21">
         <f t="shared" si="4"/>
-        <v>9.999</v>
-      </c>
-      <c r="H29" s="21">
-        <f t="shared" si="3"/>
         <v>13.332</v>
       </c>
       <c r="I29" s="19"/>
@@ -10218,11 +10226,11 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="20">
+        <f t="shared" si="5"/>
+        <v>13.332</v>
+      </c>
+      <c r="H30" s="21">
         <f t="shared" si="4"/>
-        <v>13.332</v>
-      </c>
-      <c r="H30" s="21">
-        <f t="shared" si="3"/>
         <v>16.665</v>
       </c>
       <c r="I30" s="19"/>
@@ -11421,7 +11429,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" ref="G5:G24" si="2">H4</f>
+        <f t="shared" ref="G5:G12" si="2">H4</f>
         <v>19.998</v>
       </c>
       <c r="H5" s="21">
@@ -11463,8 +11471,8 @@
       <c r="A7" s="22">
         <v>3.0</v>
       </c>
-      <c r="B7" s="17">
-        <v>4.0</v>
+      <c r="B7" s="26">
+        <v>5.0</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="17"/>
@@ -11490,8 +11498,8 @@
       <c r="A8" s="22">
         <v>4.0</v>
       </c>
-      <c r="B8" s="17">
-        <v>13.0</v>
+      <c r="B8" s="26">
+        <v>14.0</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -11507,7 +11515,7 @@
       </c>
       <c r="H8" s="21">
         <f t="shared" si="1"/>
-        <v>143.319</v>
+        <v>146.652</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>25</v>
@@ -11517,7 +11525,7 @@
       <c r="A9" s="22">
         <v>5.0</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="26">
         <v>7.0</v>
       </c>
       <c r="C9" s="18"/>
@@ -11532,11 +11540,11 @@
       </c>
       <c r="G9" s="24">
         <f t="shared" si="2"/>
-        <v>143.319</v>
+        <v>146.652</v>
       </c>
       <c r="H9" s="21">
         <f t="shared" si="1"/>
-        <v>146.652</v>
+        <v>149.985</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>113</v>
@@ -11546,7 +11554,7 @@
       <c r="A10" s="22">
         <v>6.0</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="26">
         <v>4.0</v>
       </c>
       <c r="C10" s="18"/>
@@ -11559,11 +11567,11 @@
       </c>
       <c r="G10" s="20">
         <f t="shared" si="2"/>
-        <v>146.652</v>
+        <v>149.985</v>
       </c>
       <c r="H10" s="21">
         <f t="shared" si="1"/>
-        <v>149.985</v>
+        <v>153.318</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>30</v>
@@ -11586,11 +11594,11 @@
       </c>
       <c r="G11" s="24">
         <f t="shared" si="2"/>
-        <v>149.985</v>
+        <v>153.318</v>
       </c>
       <c r="H11" s="25">
         <f t="shared" si="1"/>
-        <v>153.318</v>
+        <v>156.651</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>114</v>
@@ -11611,11 +11619,11 @@
       </c>
       <c r="G12" s="20">
         <f t="shared" si="2"/>
-        <v>153.318</v>
+        <v>156.651</v>
       </c>
       <c r="H12" s="21">
         <f t="shared" si="1"/>
-        <v>156.651</v>
+        <v>159.984</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>34</v>
@@ -11637,12 +11645,12 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="28">
-        <f t="shared" si="2"/>
-        <v>156.651</v>
+        <f>H10</f>
+        <v>153.318</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="1"/>
-        <v>159.984</v>
+        <v>156.651</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>115</v>
@@ -11664,12 +11672,12 @@
         <v>0.0</v>
       </c>
       <c r="G14" s="29">
-        <f t="shared" si="2"/>
-        <v>159.984</v>
+        <f>H13</f>
+        <v>156.651</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>
-        <v>163.317</v>
+        <v>159.984</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>41</v>
@@ -11693,12 +11701,12 @@
         <v>0.0</v>
       </c>
       <c r="G15" s="20">
-        <f t="shared" si="2"/>
-        <v>163.317</v>
+        <f>H12</f>
+        <v>159.984</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="1"/>
-        <v>166.65</v>
+        <v>163.317</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>45</v>
@@ -11720,8 +11728,8 @@
         <v>4.0</v>
       </c>
       <c r="G16" s="20">
-        <f t="shared" si="2"/>
-        <v>166.65</v>
+        <f t="shared" ref="G16:G24" si="3">H15</f>
+        <v>163.317</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="1"/>
@@ -11747,7 +11755,7 @@
         <v>0.0</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>213.312</v>
       </c>
       <c r="H17" s="25">
@@ -11774,7 +11782,7 @@
         <v>0.0</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>216.645</v>
       </c>
       <c r="H18" s="21">
@@ -11801,7 +11809,7 @@
         <v>5.0</v>
       </c>
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>219.978</v>
       </c>
       <c r="H19" s="21">
@@ -11828,7 +11836,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>246.642</v>
       </c>
       <c r="H20" s="21">
@@ -11855,7 +11863,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>249.975</v>
       </c>
       <c r="H21" s="21">
@@ -11882,7 +11890,7 @@
         <v>0.0</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>253.308</v>
       </c>
       <c r="H22" s="21">
@@ -11907,7 +11915,7 @@
         <v>6.0</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256.641</v>
       </c>
       <c r="H23" s="21">
@@ -11934,7 +11942,7 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>273.306</v>
       </c>
       <c r="H24" s="21">
@@ -11990,7 +11998,7 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="21">
-        <f t="shared" ref="H26:H30" si="3">G26+(offset($B$4,$F26,0)+1)*3.333</f>
+        <f t="shared" ref="H26:H30" si="4">G26+(offset($B$4,$F26,0)+1)*3.333</f>
         <v>3.333</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -12015,11 +12023,11 @@
         <v>0.0</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" ref="G27:G30" si="4">H26</f>
+        <f t="shared" ref="G27:G30" si="5">H26</f>
         <v>3.333</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666</v>
       </c>
       <c r="I27" s="19"/>
@@ -12040,11 +12048,11 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="20">
+        <f t="shared" si="5"/>
+        <v>6.666</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>6.666</v>
-      </c>
-      <c r="H28" s="21">
-        <f t="shared" si="3"/>
         <v>9.999</v>
       </c>
       <c r="I28" s="19"/>
@@ -12061,11 +12069,11 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="20">
+        <f t="shared" si="5"/>
+        <v>9.999</v>
+      </c>
+      <c r="H29" s="21">
         <f t="shared" si="4"/>
-        <v>9.999</v>
-      </c>
-      <c r="H29" s="21">
-        <f t="shared" si="3"/>
         <v>13.332</v>
       </c>
       <c r="I29" s="19"/>
@@ -12082,11 +12090,11 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="20">
+        <f t="shared" si="5"/>
+        <v>13.332</v>
+      </c>
+      <c r="H30" s="21">
         <f t="shared" si="4"/>
-        <v>13.332</v>
-      </c>
-      <c r="H30" s="21">
-        <f t="shared" si="3"/>
         <v>16.665</v>
       </c>
       <c r="I30" s="19"/>
@@ -13285,7 +13293,7 @@
         <v>2.0</v>
       </c>
       <c r="G5" s="21">
-        <f t="shared" ref="G5:G24" si="2">H4</f>
+        <f t="shared" ref="G5:G12" si="2">H4</f>
         <v>19.998</v>
       </c>
       <c r="H5" s="21">
@@ -13327,8 +13335,8 @@
       <c r="A7" s="22">
         <v>3.0</v>
       </c>
-      <c r="B7" s="17">
-        <v>4.0</v>
+      <c r="B7" s="26">
+        <v>5.0</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="17"/>
@@ -13354,8 +13362,8 @@
       <c r="A8" s="22">
         <v>4.0</v>
       </c>
-      <c r="B8" s="17">
-        <v>22.0</v>
+      <c r="B8" s="26">
+        <v>23.0</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
@@ -13371,7 +13379,7 @@
       </c>
       <c r="H8" s="21">
         <f t="shared" si="1"/>
-        <v>159.984</v>
+        <v>163.317</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>25</v>
@@ -13381,7 +13389,7 @@
       <c r="A9" s="22">
         <v>5.0</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="26">
         <v>7.0</v>
       </c>
       <c r="C9" s="18"/>
@@ -13396,11 +13404,11 @@
       </c>
       <c r="G9" s="25">
         <f t="shared" si="2"/>
-        <v>159.984</v>
+        <v>163.317</v>
       </c>
       <c r="H9" s="21">
         <f t="shared" si="1"/>
-        <v>163.317</v>
+        <v>166.65</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>122</v>
@@ -13410,7 +13418,7 @@
       <c r="A10" s="22">
         <v>6.0</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="26">
         <v>5.0</v>
       </c>
       <c r="C10" s="18"/>
@@ -13423,11 +13431,11 @@
       </c>
       <c r="G10" s="21">
         <f t="shared" si="2"/>
-        <v>163.317</v>
+        <v>166.65</v>
       </c>
       <c r="H10" s="21">
         <f t="shared" si="1"/>
-        <v>166.65</v>
+        <v>169.983</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>30</v>
@@ -13450,11 +13458,11 @@
       </c>
       <c r="G11" s="25">
         <f t="shared" si="2"/>
-        <v>166.65</v>
+        <v>169.983</v>
       </c>
       <c r="H11" s="25">
         <f t="shared" si="1"/>
-        <v>169.983</v>
+        <v>173.316</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>123</v>
@@ -13475,11 +13483,11 @@
       </c>
       <c r="G12" s="21">
         <f t="shared" si="2"/>
-        <v>169.983</v>
+        <v>173.316</v>
       </c>
       <c r="H12" s="21">
         <f t="shared" si="1"/>
-        <v>173.316</v>
+        <v>176.649</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>34</v>
@@ -13501,12 +13509,12 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="43">
-        <f t="shared" si="2"/>
-        <v>173.316</v>
+        <f>H10</f>
+        <v>169.983</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="1"/>
-        <v>176.649</v>
+        <v>173.316</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>124</v>
@@ -13528,12 +13536,12 @@
         <v>0.0</v>
       </c>
       <c r="G14" s="31">
-        <f t="shared" si="2"/>
-        <v>176.649</v>
+        <f>H13</f>
+        <v>173.316</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="1"/>
-        <v>179.982</v>
+        <v>176.649</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>41</v>
@@ -13557,12 +13565,12 @@
         <v>0.0</v>
       </c>
       <c r="G15" s="21">
-        <f t="shared" si="2"/>
-        <v>179.982</v>
+        <f>H12</f>
+        <v>176.649</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="1"/>
-        <v>183.315</v>
+        <v>179.982</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>45</v>
@@ -13584,8 +13592,8 @@
         <v>4.0</v>
       </c>
       <c r="G16" s="21">
-        <f t="shared" si="2"/>
-        <v>183.315</v>
+        <f t="shared" ref="G16:G24" si="3">H15</f>
+        <v>179.982</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" si="1"/>
@@ -13611,7 +13619,7 @@
         <v>0.0</v>
       </c>
       <c r="G17" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>259.974</v>
       </c>
       <c r="H17" s="25">
@@ -13638,7 +13646,7 @@
         <v>0.0</v>
       </c>
       <c r="G18" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>263.307</v>
       </c>
       <c r="H18" s="21">
@@ -13665,7 +13673,7 @@
         <v>5.0</v>
       </c>
       <c r="G19" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>266.64</v>
       </c>
       <c r="H19" s="21">
@@ -13692,7 +13700,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>293.304</v>
       </c>
       <c r="H20" s="21">
@@ -13719,7 +13727,7 @@
         <v>0.0</v>
       </c>
       <c r="G21" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>296.637</v>
       </c>
       <c r="H21" s="21">
@@ -13746,7 +13754,7 @@
         <v>0.0</v>
       </c>
       <c r="G22" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>299.97</v>
       </c>
       <c r="H22" s="21">
@@ -13771,7 +13779,7 @@
         <v>6.0</v>
       </c>
       <c r="G23" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>303.303</v>
       </c>
       <c r="H23" s="21">
@@ -13798,7 +13806,7 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>323.301</v>
       </c>
       <c r="H24" s="21">
@@ -13854,7 +13862,7 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="21">
-        <f t="shared" ref="H26:H30" si="3">G26+(offset($B$4,$F26,0)+1)*3.333</f>
+        <f t="shared" ref="H26:H30" si="4">G26+(offset($B$4,$F26,0)+1)*3.333</f>
         <v>3.333</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -13879,11 +13887,11 @@
         <v>0.0</v>
       </c>
       <c r="G27" s="21">
-        <f t="shared" ref="G27:G30" si="4">H26</f>
+        <f t="shared" ref="G27:G30" si="5">H26</f>
         <v>3.333</v>
       </c>
       <c r="H27" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666</v>
       </c>
       <c r="I27" s="19"/>
@@ -13904,11 +13912,11 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="21">
+        <f t="shared" si="5"/>
+        <v>6.666</v>
+      </c>
+      <c r="H28" s="21">
         <f t="shared" si="4"/>
-        <v>6.666</v>
-      </c>
-      <c r="H28" s="21">
-        <f t="shared" si="3"/>
         <v>9.999</v>
       </c>
       <c r="I28" s="19"/>
@@ -13925,11 +13933,11 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="21">
+        <f t="shared" si="5"/>
+        <v>9.999</v>
+      </c>
+      <c r="H29" s="21">
         <f t="shared" si="4"/>
-        <v>9.999</v>
-      </c>
-      <c r="H29" s="21">
-        <f t="shared" si="3"/>
         <v>13.332</v>
       </c>
       <c r="I29" s="19"/>
@@ -13946,11 +13954,11 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="21">
+        <f t="shared" si="5"/>
+        <v>13.332</v>
+      </c>
+      <c r="H30" s="21">
         <f t="shared" si="4"/>
-        <v>13.332</v>
-      </c>
-      <c r="H30" s="21">
-        <f t="shared" si="3"/>
         <v>16.665</v>
       </c>
       <c r="I30" s="19"/>

</xml_diff>